<commit_message>
purwin report files and csv excel file with more detailed analysis.
</commit_message>
<xml_diff>
--- a/Soupfm-Analise(P220125_0011)/PurgePrémiosTotobolaExtra_analise.xlsx
+++ b/Soupfm-Analise(P220125_0011)/PurgePrémiosTotobolaExtra_analise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\Soupfm-Analise(P220125_0011)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931A887B-2B68-48C2-A512-0AEA0E5410F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D495F9-2E95-4DDB-BE57-C0032683E4BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="304" firstSheet="1" activeTab="2" xr2:uid="{89E42766-7B63-4A9C-830B-B7B71F3C9249}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="304" firstSheet="1" activeTab="1" xr2:uid="{89E42766-7B63-4A9C-830B-B7B71F3C9249}"/>
   </bookViews>
   <sheets>
     <sheet name="Analise preleminares" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>Data Escrutínio</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Total Registos</t>
+  </si>
+  <si>
+    <t>dia antes de gerar o upurge</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +226,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -236,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -257,9 +266,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -274,6 +280,14 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,8 +629,8 @@
       <xdr:rowOff>11906</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>517555</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>29399</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>2885</xdr:rowOff>
     </xdr:to>
@@ -659,8 +673,8 @@
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>7144</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>126206</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>109974</xdr:rowOff>
     </xdr:to>
@@ -1228,6 +1242,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>610913</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>472327</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>162719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39C92F47-C7C1-4501-ADFC-554C0F6005DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7731672" y="6286500"/>
+          <a:ext cx="7192379" cy="5687219"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2037,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FC5992-8E59-4CD7-AAC7-1656CA4A1D7F}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="N31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,6 +2116,7 @@
     <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -2226,6 +2285,9 @@
         <f>M6-$D$2+1</f>
         <v>7583</v>
       </c>
+      <c r="R6" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2267,6 +2329,12 @@
       <c r="N7" s="3">
         <f>M7-$D$2+1</f>
         <v>7569</v>
+      </c>
+      <c r="R7" s="16">
+        <v>44627</v>
+      </c>
+      <c r="S7" s="18">
+        <v>7616</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2363,20 +2431,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B052328-7EEA-4BBC-9302-968DCCA8FD0A}">
   <dimension ref="B25:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2384,7 +2452,7 @@
       <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>20220308</v>
       </c>
     </row>
@@ -2392,7 +2460,7 @@
       <c r="B27" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>20220311</v>
       </c>
     </row>
@@ -2400,7 +2468,7 @@
       <c r="B60" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="14">
+      <c r="C60" s="13">
         <v>1</v>
       </c>
       <c r="D60" s="9" t="s">
@@ -2413,35 +2481,35 @@
       <c r="B61" t="s">
         <v>37</v>
       </c>
-      <c r="C61" s="12">
+      <c r="C61" s="11">
         <v>10</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E61" s="10"/>
+      <c r="E61" s="17"/>
       <c r="F61" s="9"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>38</v>
       </c>
-      <c r="C62" s="12">
+      <c r="C62" s="11">
         <v>7525003105178</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="64" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="12" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2449,7 +2517,7 @@
       <c r="B83" t="s">
         <v>35</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D83" t="s">
@@ -2460,7 +2528,7 @@
       <c r="B84" t="s">
         <v>37</v>
       </c>
-      <c r="C84" s="12">
+      <c r="C84" s="11">
         <v>9</v>
       </c>
       <c r="D84" t="s">

</xml_diff>